<commit_message>
Epid data and structure edited
</commit_message>
<xml_diff>
--- a/data/chelyabinsk/pcr.xlsx
+++ b/data/chelyabinsk/pcr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrey/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4FFD51-4C16-984F-A6B0-7AA5F1E64EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C1AF37-AD6C-004C-8532-2BE4CD216B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B385EF63-4861-4686-B598-593F69A2DF0D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{B385EF63-4861-4686-B598-593F69A2DF0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Челябинск" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="790">
   <si>
     <t>Число образцов тестированных на грипп</t>
   </si>
@@ -11169,6 +11169,549 @@
         <charset val="204"/>
       </rPr>
       <t> (04.03.2024 - 10.03.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (11.03.2024 - 17.03.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (18.03.2024 - 24.03.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (25.03.2024 - 31.03.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (01.04.2024 - 07.04.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (08.04.2024 - 14.04.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (15.04.2024 - 21.04.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (22.04.2024 - 28.04.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (29.04.2024 - 05.05.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (06.05.2024 - 12.05.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (13.05.2024 - 19.05.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (20.05.2024 - 26.05.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.22</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (27.05.2024 - 02.06.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (03.06.2024 - 09.06.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (10.06.2024 - 16.06.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.25</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (17.06.2024 - 23.06.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.26</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (24.06.2024 - 30.06.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.27</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (01.07.2024 - 07.07.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.28</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (08.07.2024 - 14.07.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.29</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (15.07.2024 - 21.07.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (22.07.2024 - 28.07.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.31</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (29.07.2024 - 04.08.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.32</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (05.08.2024 - 11.08.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.33</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (12.08.2024 - 18.08.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (19.08.2024 - 25.08.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.35</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (26.08.2024 - 01.09.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.36</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (02.09.2024 - 08.09.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.37</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (09.09.2024 - 15.09.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.38</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (16.09.2024 - 22.09.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.39</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (23.09.2024 - 29.09.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (30.09.2024 - 06.10.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.41</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (07.10.2024 - 13.10.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.42</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (14.10.2024 - 20.10.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> (21.10.2024 - 27.10.2024)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2024.44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t> (28.10.2024 - 03.11.2024)</t>
     </r>
   </si>
   <si>
@@ -11179,7 +11722,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -11211,6 +11754,46 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -11232,7 +11815,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -11358,11 +11941,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF1428A1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF1428A1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11388,6 +11982,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11702,9 +12312,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9865F2A7-57BB-4A8F-88F9-71CC1269A5CC}">
-  <dimension ref="A1:P742"/>
+  <dimension ref="A1:P776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11713,7 +12325,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="122" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>755</v>
+        <v>789</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -39909,7 +40521,1437 @@
         <v>17</v>
       </c>
     </row>
-    <row r="742" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="742" spans="1:16" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A742" s="9" t="s">
+        <v>755</v>
+      </c>
+      <c r="B742" s="10">
+        <v>222</v>
+      </c>
+      <c r="C742" s="10">
+        <v>0</v>
+      </c>
+      <c r="D742" s="10">
+        <v>0</v>
+      </c>
+      <c r="E742" s="10">
+        <v>3</v>
+      </c>
+      <c r="F742" s="10">
+        <v>0</v>
+      </c>
+      <c r="G742" s="10">
+        <v>222</v>
+      </c>
+      <c r="H742" s="10">
+        <v>5</v>
+      </c>
+      <c r="I742" s="10">
+        <v>3</v>
+      </c>
+      <c r="J742" s="10">
+        <v>40</v>
+      </c>
+      <c r="K742" s="10">
+        <v>7</v>
+      </c>
+      <c r="L742" s="10">
+        <v>5</v>
+      </c>
+      <c r="M742" s="10">
+        <v>5</v>
+      </c>
+      <c r="N742" s="10">
+        <v>4</v>
+      </c>
+      <c r="O742" s="10">
+        <v>222</v>
+      </c>
+      <c r="P742" s="11">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="743" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A743" s="9" t="s">
+        <v>756</v>
+      </c>
+      <c r="B743" s="10"/>
+      <c r="C743" s="10"/>
+      <c r="D743" s="10"/>
+      <c r="E743" s="10"/>
+      <c r="F743" s="10"/>
+      <c r="G743" s="10"/>
+      <c r="H743" s="10"/>
+      <c r="I743" s="10"/>
+      <c r="J743" s="10"/>
+      <c r="K743" s="10"/>
+      <c r="L743" s="10"/>
+      <c r="M743" s="10"/>
+      <c r="N743" s="10"/>
+      <c r="O743" s="10"/>
+      <c r="P743" s="11"/>
+    </row>
+    <row r="744" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A744" s="9" t="s">
+        <v>757</v>
+      </c>
+      <c r="B744" s="10"/>
+      <c r="C744" s="10"/>
+      <c r="D744" s="10"/>
+      <c r="E744" s="10"/>
+      <c r="F744" s="10"/>
+      <c r="G744" s="10"/>
+      <c r="H744" s="10"/>
+      <c r="I744" s="10"/>
+      <c r="J744" s="10"/>
+      <c r="K744" s="10"/>
+      <c r="L744" s="10"/>
+      <c r="M744" s="10"/>
+      <c r="N744" s="10"/>
+      <c r="O744" s="10"/>
+      <c r="P744" s="11"/>
+    </row>
+    <row r="745" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A745" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="B745" s="10"/>
+      <c r="C745" s="10"/>
+      <c r="D745" s="10"/>
+      <c r="E745" s="10"/>
+      <c r="F745" s="10"/>
+      <c r="G745" s="10"/>
+      <c r="H745" s="10"/>
+      <c r="I745" s="10"/>
+      <c r="J745" s="10"/>
+      <c r="K745" s="10"/>
+      <c r="L745" s="10"/>
+      <c r="M745" s="10"/>
+      <c r="N745" s="10"/>
+      <c r="O745" s="10"/>
+      <c r="P745" s="11"/>
+    </row>
+    <row r="746" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A746" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="B746" s="10"/>
+      <c r="C746" s="10"/>
+      <c r="D746" s="10"/>
+      <c r="E746" s="10"/>
+      <c r="F746" s="10"/>
+      <c r="G746" s="10"/>
+      <c r="H746" s="10"/>
+      <c r="I746" s="10"/>
+      <c r="J746" s="10"/>
+      <c r="K746" s="10"/>
+      <c r="L746" s="10"/>
+      <c r="M746" s="10"/>
+      <c r="N746" s="10"/>
+      <c r="O746" s="10"/>
+      <c r="P746" s="11"/>
+    </row>
+    <row r="747" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A747" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="B747" s="10">
+        <v>129</v>
+      </c>
+      <c r="C747" s="10">
+        <v>0</v>
+      </c>
+      <c r="D747" s="10">
+        <v>0</v>
+      </c>
+      <c r="E747" s="10">
+        <v>0</v>
+      </c>
+      <c r="F747" s="10">
+        <v>1</v>
+      </c>
+      <c r="G747" s="10">
+        <v>129</v>
+      </c>
+      <c r="H747" s="10">
+        <v>7</v>
+      </c>
+      <c r="I747" s="10">
+        <v>3</v>
+      </c>
+      <c r="J747" s="10">
+        <v>4</v>
+      </c>
+      <c r="K747" s="10">
+        <v>20</v>
+      </c>
+      <c r="L747" s="10">
+        <v>5</v>
+      </c>
+      <c r="M747" s="10">
+        <v>0</v>
+      </c>
+      <c r="N747" s="10">
+        <v>0</v>
+      </c>
+      <c r="O747" s="10">
+        <v>129</v>
+      </c>
+      <c r="P747" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="748" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A748" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="B748" s="10"/>
+      <c r="C748" s="10"/>
+      <c r="D748" s="10"/>
+      <c r="E748" s="10"/>
+      <c r="F748" s="10"/>
+      <c r="G748" s="10"/>
+      <c r="H748" s="10"/>
+      <c r="I748" s="10"/>
+      <c r="J748" s="10"/>
+      <c r="K748" s="10"/>
+      <c r="L748" s="10"/>
+      <c r="M748" s="10"/>
+      <c r="N748" s="10"/>
+      <c r="O748" s="10"/>
+      <c r="P748" s="11"/>
+    </row>
+    <row r="749" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A749" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="B749" s="10">
+        <v>51</v>
+      </c>
+      <c r="C749" s="10">
+        <v>0</v>
+      </c>
+      <c r="D749" s="10">
+        <v>0</v>
+      </c>
+      <c r="E749" s="10">
+        <v>0</v>
+      </c>
+      <c r="F749" s="10">
+        <v>2</v>
+      </c>
+      <c r="G749" s="10">
+        <v>51</v>
+      </c>
+      <c r="H749" s="10">
+        <v>5</v>
+      </c>
+      <c r="I749" s="10">
+        <v>1</v>
+      </c>
+      <c r="J749" s="10">
+        <v>1</v>
+      </c>
+      <c r="K749" s="10">
+        <v>7</v>
+      </c>
+      <c r="L749" s="10">
+        <v>0</v>
+      </c>
+      <c r="M749" s="10">
+        <v>1</v>
+      </c>
+      <c r="N749" s="10">
+        <v>4</v>
+      </c>
+      <c r="O749" s="10">
+        <v>51</v>
+      </c>
+      <c r="P749" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="750" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A750" s="9" t="s">
+        <v>763</v>
+      </c>
+      <c r="B750" s="10">
+        <v>142</v>
+      </c>
+      <c r="C750" s="10">
+        <v>0</v>
+      </c>
+      <c r="D750" s="10">
+        <v>0</v>
+      </c>
+      <c r="E750" s="10">
+        <v>0</v>
+      </c>
+      <c r="F750" s="10">
+        <v>2</v>
+      </c>
+      <c r="G750" s="10">
+        <v>142</v>
+      </c>
+      <c r="H750" s="10">
+        <v>6</v>
+      </c>
+      <c r="I750" s="10">
+        <v>1</v>
+      </c>
+      <c r="J750" s="10">
+        <v>2</v>
+      </c>
+      <c r="K750" s="10">
+        <v>19</v>
+      </c>
+      <c r="L750" s="10">
+        <v>5</v>
+      </c>
+      <c r="M750" s="10">
+        <v>2</v>
+      </c>
+      <c r="N750" s="10">
+        <v>0</v>
+      </c>
+      <c r="O750" s="10">
+        <v>142</v>
+      </c>
+      <c r="P750" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="751" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A751" s="9" t="s">
+        <v>764</v>
+      </c>
+      <c r="B751" s="10">
+        <v>93</v>
+      </c>
+      <c r="C751" s="10">
+        <v>0</v>
+      </c>
+      <c r="D751" s="10">
+        <v>0</v>
+      </c>
+      <c r="E751" s="10">
+        <v>0</v>
+      </c>
+      <c r="F751" s="10">
+        <v>5</v>
+      </c>
+      <c r="G751" s="10">
+        <v>93</v>
+      </c>
+      <c r="H751" s="10">
+        <v>3</v>
+      </c>
+      <c r="I751" s="10">
+        <v>0</v>
+      </c>
+      <c r="J751" s="10">
+        <v>0</v>
+      </c>
+      <c r="K751" s="10">
+        <v>17</v>
+      </c>
+      <c r="L751" s="10">
+        <v>0</v>
+      </c>
+      <c r="M751" s="10">
+        <v>0</v>
+      </c>
+      <c r="N751" s="10">
+        <v>1</v>
+      </c>
+      <c r="O751" s="10">
+        <v>93</v>
+      </c>
+      <c r="P751" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="752" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A752" s="9" t="s">
+        <v>765</v>
+      </c>
+      <c r="B752" s="10">
+        <v>81</v>
+      </c>
+      <c r="C752" s="10">
+        <v>0</v>
+      </c>
+      <c r="D752" s="10">
+        <v>0</v>
+      </c>
+      <c r="E752" s="10">
+        <v>0</v>
+      </c>
+      <c r="F752" s="10">
+        <v>0</v>
+      </c>
+      <c r="G752" s="10">
+        <v>81</v>
+      </c>
+      <c r="H752" s="10">
+        <v>4</v>
+      </c>
+      <c r="I752" s="10">
+        <v>1</v>
+      </c>
+      <c r="J752" s="10">
+        <v>0</v>
+      </c>
+      <c r="K752" s="10">
+        <v>14</v>
+      </c>
+      <c r="L752" s="10">
+        <v>1</v>
+      </c>
+      <c r="M752" s="10">
+        <v>1</v>
+      </c>
+      <c r="N752" s="10">
+        <v>1</v>
+      </c>
+      <c r="O752" s="10">
+        <v>81</v>
+      </c>
+      <c r="P752" s="11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="753" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A753" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="B753" s="10">
+        <v>181</v>
+      </c>
+      <c r="C753" s="10">
+        <v>0</v>
+      </c>
+      <c r="D753" s="10">
+        <v>0</v>
+      </c>
+      <c r="E753" s="10">
+        <v>0</v>
+      </c>
+      <c r="F753" s="10">
+        <v>4</v>
+      </c>
+      <c r="G753" s="10">
+        <v>181</v>
+      </c>
+      <c r="H753" s="10">
+        <v>8</v>
+      </c>
+      <c r="I753" s="10">
+        <v>2</v>
+      </c>
+      <c r="J753" s="10">
+        <v>0</v>
+      </c>
+      <c r="K753" s="10">
+        <v>32</v>
+      </c>
+      <c r="L753" s="10">
+        <v>0</v>
+      </c>
+      <c r="M753" s="10">
+        <v>0</v>
+      </c>
+      <c r="N753" s="10">
+        <v>2</v>
+      </c>
+      <c r="O753" s="10">
+        <v>181</v>
+      </c>
+      <c r="P753" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="754" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A754" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="B754" s="10">
+        <v>232</v>
+      </c>
+      <c r="C754" s="10">
+        <v>0</v>
+      </c>
+      <c r="D754" s="10">
+        <v>0</v>
+      </c>
+      <c r="E754" s="10">
+        <v>0</v>
+      </c>
+      <c r="F754" s="10">
+        <v>2</v>
+      </c>
+      <c r="G754" s="10">
+        <v>232</v>
+      </c>
+      <c r="H754" s="10">
+        <v>8</v>
+      </c>
+      <c r="I754" s="10">
+        <v>4</v>
+      </c>
+      <c r="J754" s="10">
+        <v>0</v>
+      </c>
+      <c r="K754" s="10">
+        <v>33</v>
+      </c>
+      <c r="L754" s="10">
+        <v>2</v>
+      </c>
+      <c r="M754" s="10">
+        <v>0</v>
+      </c>
+      <c r="N754" s="10">
+        <v>0</v>
+      </c>
+      <c r="O754" s="10">
+        <v>232</v>
+      </c>
+      <c r="P754" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="755" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A755" s="9" t="s">
+        <v>768</v>
+      </c>
+      <c r="B755" s="10">
+        <v>177</v>
+      </c>
+      <c r="C755" s="10">
+        <v>0</v>
+      </c>
+      <c r="D755" s="10">
+        <v>0</v>
+      </c>
+      <c r="E755" s="10">
+        <v>0</v>
+      </c>
+      <c r="F755" s="10">
+        <v>2</v>
+      </c>
+      <c r="G755" s="10">
+        <v>177</v>
+      </c>
+      <c r="H755" s="10">
+        <v>11</v>
+      </c>
+      <c r="I755" s="10">
+        <v>6</v>
+      </c>
+      <c r="J755" s="10">
+        <v>1</v>
+      </c>
+      <c r="K755" s="10">
+        <v>33</v>
+      </c>
+      <c r="L755" s="10">
+        <v>1</v>
+      </c>
+      <c r="M755" s="10">
+        <v>0</v>
+      </c>
+      <c r="N755" s="10">
+        <v>1</v>
+      </c>
+      <c r="O755" s="10">
+        <v>177</v>
+      </c>
+      <c r="P755" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="756" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A756" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="B756" s="10">
+        <v>162</v>
+      </c>
+      <c r="C756" s="10">
+        <v>0</v>
+      </c>
+      <c r="D756" s="10">
+        <v>0</v>
+      </c>
+      <c r="E756" s="10">
+        <v>0</v>
+      </c>
+      <c r="F756" s="10">
+        <v>1</v>
+      </c>
+      <c r="G756" s="10">
+        <v>162</v>
+      </c>
+      <c r="H756" s="10">
+        <v>8</v>
+      </c>
+      <c r="I756" s="10">
+        <v>3</v>
+      </c>
+      <c r="J756" s="10">
+        <v>0</v>
+      </c>
+      <c r="K756" s="10">
+        <v>16</v>
+      </c>
+      <c r="L756" s="10">
+        <v>0</v>
+      </c>
+      <c r="M756" s="10">
+        <v>0</v>
+      </c>
+      <c r="N756" s="10">
+        <v>1</v>
+      </c>
+      <c r="O756" s="10">
+        <v>162</v>
+      </c>
+      <c r="P756" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="757" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A757" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="B757" s="10">
+        <v>137</v>
+      </c>
+      <c r="C757" s="10">
+        <v>0</v>
+      </c>
+      <c r="D757" s="10">
+        <v>0</v>
+      </c>
+      <c r="E757" s="10">
+        <v>0</v>
+      </c>
+      <c r="F757" s="10">
+        <v>0</v>
+      </c>
+      <c r="G757" s="10">
+        <v>137</v>
+      </c>
+      <c r="H757" s="10">
+        <v>7</v>
+      </c>
+      <c r="I757" s="10">
+        <v>2</v>
+      </c>
+      <c r="J757" s="10">
+        <v>0</v>
+      </c>
+      <c r="K757" s="10">
+        <v>12</v>
+      </c>
+      <c r="L757" s="10">
+        <v>0</v>
+      </c>
+      <c r="M757" s="10">
+        <v>0</v>
+      </c>
+      <c r="N757" s="10">
+        <v>0</v>
+      </c>
+      <c r="O757" s="10">
+        <v>137</v>
+      </c>
+      <c r="P757" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="758" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A758" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="B758" s="10">
+        <v>184</v>
+      </c>
+      <c r="C758" s="10">
+        <v>0</v>
+      </c>
+      <c r="D758" s="10">
+        <v>0</v>
+      </c>
+      <c r="E758" s="10">
+        <v>0</v>
+      </c>
+      <c r="F758" s="10">
+        <v>1</v>
+      </c>
+      <c r="G758" s="10">
+        <v>184</v>
+      </c>
+      <c r="H758" s="10">
+        <v>8</v>
+      </c>
+      <c r="I758" s="10">
+        <v>9</v>
+      </c>
+      <c r="J758" s="10">
+        <v>0</v>
+      </c>
+      <c r="K758" s="10">
+        <v>12</v>
+      </c>
+      <c r="L758" s="10">
+        <v>1</v>
+      </c>
+      <c r="M758" s="10">
+        <v>0</v>
+      </c>
+      <c r="N758" s="10">
+        <v>0</v>
+      </c>
+      <c r="O758" s="10">
+        <v>184</v>
+      </c>
+      <c r="P758" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="759" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A759" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="B759" s="10">
+        <v>245</v>
+      </c>
+      <c r="C759" s="10">
+        <v>0</v>
+      </c>
+      <c r="D759" s="10">
+        <v>0</v>
+      </c>
+      <c r="E759" s="10">
+        <v>1</v>
+      </c>
+      <c r="F759" s="10">
+        <v>1</v>
+      </c>
+      <c r="G759" s="10">
+        <v>245</v>
+      </c>
+      <c r="H759" s="10">
+        <v>8</v>
+      </c>
+      <c r="I759" s="10">
+        <v>6</v>
+      </c>
+      <c r="J759" s="10">
+        <v>0</v>
+      </c>
+      <c r="K759" s="10">
+        <v>27</v>
+      </c>
+      <c r="L759" s="10">
+        <v>0</v>
+      </c>
+      <c r="M759" s="10">
+        <v>0</v>
+      </c>
+      <c r="N759" s="10">
+        <v>2</v>
+      </c>
+      <c r="O759" s="10">
+        <v>245</v>
+      </c>
+      <c r="P759" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="760" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A760" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="B760" s="10">
+        <v>211</v>
+      </c>
+      <c r="C760" s="10">
+        <v>0</v>
+      </c>
+      <c r="D760" s="10">
+        <v>0</v>
+      </c>
+      <c r="E760" s="10">
+        <v>0</v>
+      </c>
+      <c r="F760" s="10">
+        <v>0</v>
+      </c>
+      <c r="G760" s="10">
+        <v>211</v>
+      </c>
+      <c r="H760" s="10">
+        <v>8</v>
+      </c>
+      <c r="I760" s="10">
+        <v>5</v>
+      </c>
+      <c r="J760" s="10">
+        <v>0</v>
+      </c>
+      <c r="K760" s="10">
+        <v>20</v>
+      </c>
+      <c r="L760" s="10">
+        <v>0</v>
+      </c>
+      <c r="M760" s="10">
+        <v>1</v>
+      </c>
+      <c r="N760" s="10">
+        <v>0</v>
+      </c>
+      <c r="O760" s="10">
+        <v>211</v>
+      </c>
+      <c r="P760" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="761" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A761" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="B761" s="10">
+        <v>214</v>
+      </c>
+      <c r="C761" s="10">
+        <v>0</v>
+      </c>
+      <c r="D761" s="10">
+        <v>0</v>
+      </c>
+      <c r="E761" s="10">
+        <v>0</v>
+      </c>
+      <c r="F761" s="10">
+        <v>0</v>
+      </c>
+      <c r="G761" s="10">
+        <v>214</v>
+      </c>
+      <c r="H761" s="10">
+        <v>2</v>
+      </c>
+      <c r="I761" s="10">
+        <v>6</v>
+      </c>
+      <c r="J761" s="10">
+        <v>0</v>
+      </c>
+      <c r="K761" s="10">
+        <v>17</v>
+      </c>
+      <c r="L761" s="10">
+        <v>0</v>
+      </c>
+      <c r="M761" s="10">
+        <v>0</v>
+      </c>
+      <c r="N761" s="10">
+        <v>2</v>
+      </c>
+      <c r="O761" s="10">
+        <v>214</v>
+      </c>
+      <c r="P761" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="762" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A762" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="B762" s="10">
+        <v>178</v>
+      </c>
+      <c r="C762" s="10">
+        <v>0</v>
+      </c>
+      <c r="D762" s="10">
+        <v>0</v>
+      </c>
+      <c r="E762" s="10">
+        <v>0</v>
+      </c>
+      <c r="F762" s="10">
+        <v>0</v>
+      </c>
+      <c r="G762" s="10">
+        <v>178</v>
+      </c>
+      <c r="H762" s="10">
+        <v>2</v>
+      </c>
+      <c r="I762" s="10">
+        <v>0</v>
+      </c>
+      <c r="J762" s="10">
+        <v>0</v>
+      </c>
+      <c r="K762" s="10">
+        <v>23</v>
+      </c>
+      <c r="L762" s="10">
+        <v>0</v>
+      </c>
+      <c r="M762" s="10">
+        <v>0</v>
+      </c>
+      <c r="N762" s="10">
+        <v>0</v>
+      </c>
+      <c r="O762" s="10">
+        <v>178</v>
+      </c>
+      <c r="P762" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A763" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="B763" s="10">
+        <v>209</v>
+      </c>
+      <c r="C763" s="10">
+        <v>0</v>
+      </c>
+      <c r="D763" s="10">
+        <v>0</v>
+      </c>
+      <c r="E763" s="10">
+        <v>0</v>
+      </c>
+      <c r="F763" s="10">
+        <v>0</v>
+      </c>
+      <c r="G763" s="10">
+        <v>209</v>
+      </c>
+      <c r="H763" s="10">
+        <v>6</v>
+      </c>
+      <c r="I763" s="10">
+        <v>1</v>
+      </c>
+      <c r="J763" s="10">
+        <v>0</v>
+      </c>
+      <c r="K763" s="10">
+        <v>40</v>
+      </c>
+      <c r="L763" s="10">
+        <v>1</v>
+      </c>
+      <c r="M763" s="10">
+        <v>0</v>
+      </c>
+      <c r="N763" s="10">
+        <v>3</v>
+      </c>
+      <c r="O763" s="10">
+        <v>209</v>
+      </c>
+      <c r="P763" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="764" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A764" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="B764" s="10">
+        <v>245</v>
+      </c>
+      <c r="C764" s="10">
+        <v>0</v>
+      </c>
+      <c r="D764" s="10">
+        <v>0</v>
+      </c>
+      <c r="E764" s="10">
+        <v>0</v>
+      </c>
+      <c r="F764" s="10">
+        <v>0</v>
+      </c>
+      <c r="G764" s="10">
+        <v>245</v>
+      </c>
+      <c r="H764" s="10">
+        <v>9</v>
+      </c>
+      <c r="I764" s="10">
+        <v>3</v>
+      </c>
+      <c r="J764" s="10">
+        <v>0</v>
+      </c>
+      <c r="K764" s="10">
+        <v>36</v>
+      </c>
+      <c r="L764" s="10">
+        <v>0</v>
+      </c>
+      <c r="M764" s="10">
+        <v>0</v>
+      </c>
+      <c r="N764" s="10">
+        <v>2</v>
+      </c>
+      <c r="O764" s="10">
+        <v>245</v>
+      </c>
+      <c r="P764" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="765" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A765" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="B765" s="10">
+        <v>289</v>
+      </c>
+      <c r="C765" s="10">
+        <v>0</v>
+      </c>
+      <c r="D765" s="10">
+        <v>0</v>
+      </c>
+      <c r="E765" s="10">
+        <v>0</v>
+      </c>
+      <c r="F765" s="10">
+        <v>0</v>
+      </c>
+      <c r="G765" s="10">
+        <v>289</v>
+      </c>
+      <c r="H765" s="10">
+        <v>18</v>
+      </c>
+      <c r="I765" s="10">
+        <v>3</v>
+      </c>
+      <c r="J765" s="10">
+        <v>0</v>
+      </c>
+      <c r="K765" s="10">
+        <v>53</v>
+      </c>
+      <c r="L765" s="10">
+        <v>0</v>
+      </c>
+      <c r="M765" s="10">
+        <v>0</v>
+      </c>
+      <c r="N765" s="10">
+        <v>9</v>
+      </c>
+      <c r="O765" s="10">
+        <v>212</v>
+      </c>
+      <c r="P765" s="11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="766" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A766" s="9" t="s">
+        <v>779</v>
+      </c>
+      <c r="B766" s="10">
+        <v>253</v>
+      </c>
+      <c r="C766" s="10">
+        <v>0</v>
+      </c>
+      <c r="D766" s="10">
+        <v>0</v>
+      </c>
+      <c r="E766" s="10">
+        <v>0</v>
+      </c>
+      <c r="F766" s="10">
+        <v>0</v>
+      </c>
+      <c r="G766" s="10">
+        <v>253</v>
+      </c>
+      <c r="H766" s="10">
+        <v>6</v>
+      </c>
+      <c r="I766" s="10">
+        <v>2</v>
+      </c>
+      <c r="J766" s="10">
+        <v>0</v>
+      </c>
+      <c r="K766" s="10">
+        <v>28</v>
+      </c>
+      <c r="L766" s="10">
+        <v>0</v>
+      </c>
+      <c r="M766" s="10">
+        <v>0</v>
+      </c>
+      <c r="N766" s="10">
+        <v>2</v>
+      </c>
+      <c r="O766" s="10">
+        <v>253</v>
+      </c>
+      <c r="P766" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="767" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A767" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="B767" s="10">
+        <v>258</v>
+      </c>
+      <c r="C767" s="10">
+        <v>0</v>
+      </c>
+      <c r="D767" s="10">
+        <v>0</v>
+      </c>
+      <c r="E767" s="10">
+        <v>0</v>
+      </c>
+      <c r="F767" s="10">
+        <v>0</v>
+      </c>
+      <c r="G767" s="10">
+        <v>258</v>
+      </c>
+      <c r="H767" s="10">
+        <v>6</v>
+      </c>
+      <c r="I767" s="10">
+        <v>3</v>
+      </c>
+      <c r="J767" s="10">
+        <v>1</v>
+      </c>
+      <c r="K767" s="10">
+        <v>37</v>
+      </c>
+      <c r="L767" s="10">
+        <v>0</v>
+      </c>
+      <c r="M767" s="10">
+        <v>0</v>
+      </c>
+      <c r="N767" s="10">
+        <v>2</v>
+      </c>
+      <c r="O767" s="10">
+        <v>258</v>
+      </c>
+      <c r="P767" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="768" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A768" s="9" t="s">
+        <v>781</v>
+      </c>
+      <c r="B768" s="10">
+        <v>272</v>
+      </c>
+      <c r="C768" s="10">
+        <v>0</v>
+      </c>
+      <c r="D768" s="10">
+        <v>0</v>
+      </c>
+      <c r="E768" s="10">
+        <v>0</v>
+      </c>
+      <c r="F768" s="10">
+        <v>0</v>
+      </c>
+      <c r="G768" s="10">
+        <v>272</v>
+      </c>
+      <c r="H768" s="10">
+        <v>9</v>
+      </c>
+      <c r="I768" s="10">
+        <v>23</v>
+      </c>
+      <c r="J768" s="10">
+        <v>4</v>
+      </c>
+      <c r="K768" s="10">
+        <v>35</v>
+      </c>
+      <c r="L768" s="10">
+        <v>0</v>
+      </c>
+      <c r="M768" s="10">
+        <v>1</v>
+      </c>
+      <c r="N768" s="10">
+        <v>0</v>
+      </c>
+      <c r="O768" s="10">
+        <v>272</v>
+      </c>
+      <c r="P768" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="769" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A769" s="9" t="s">
+        <v>782</v>
+      </c>
+      <c r="B769" s="10">
+        <v>331</v>
+      </c>
+      <c r="C769" s="10">
+        <v>0</v>
+      </c>
+      <c r="D769" s="10">
+        <v>0</v>
+      </c>
+      <c r="E769" s="10">
+        <v>0</v>
+      </c>
+      <c r="F769" s="10">
+        <v>0</v>
+      </c>
+      <c r="G769" s="10">
+        <v>331</v>
+      </c>
+      <c r="H769" s="10">
+        <v>6</v>
+      </c>
+      <c r="I769" s="10">
+        <v>7</v>
+      </c>
+      <c r="J769" s="10">
+        <v>0</v>
+      </c>
+      <c r="K769" s="10">
+        <v>55</v>
+      </c>
+      <c r="L769" s="10">
+        <v>1</v>
+      </c>
+      <c r="M769" s="10">
+        <v>1</v>
+      </c>
+      <c r="N769" s="10">
+        <v>5</v>
+      </c>
+      <c r="O769" s="10">
+        <v>331</v>
+      </c>
+      <c r="P769" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="770" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A770" s="9" t="s">
+        <v>783</v>
+      </c>
+      <c r="B770" s="10"/>
+      <c r="C770" s="10"/>
+      <c r="D770" s="10"/>
+      <c r="E770" s="10"/>
+      <c r="F770" s="10"/>
+      <c r="G770" s="10"/>
+      <c r="H770" s="10"/>
+      <c r="I770" s="10"/>
+      <c r="J770" s="10"/>
+      <c r="K770" s="10"/>
+      <c r="L770" s="10"/>
+      <c r="M770" s="10"/>
+      <c r="N770" s="10"/>
+      <c r="O770" s="10"/>
+      <c r="P770" s="11"/>
+    </row>
+    <row r="771" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A771" s="9" t="s">
+        <v>784</v>
+      </c>
+      <c r="B771" s="10"/>
+      <c r="C771" s="10"/>
+      <c r="D771" s="10"/>
+      <c r="E771" s="10"/>
+      <c r="F771" s="10"/>
+      <c r="G771" s="10"/>
+      <c r="H771" s="10"/>
+      <c r="I771" s="10"/>
+      <c r="J771" s="10"/>
+      <c r="K771" s="10"/>
+      <c r="L771" s="10"/>
+      <c r="M771" s="10"/>
+      <c r="N771" s="10"/>
+      <c r="O771" s="10"/>
+      <c r="P771" s="11"/>
+    </row>
+    <row r="772" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A772" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="B772" s="10">
+        <v>301</v>
+      </c>
+      <c r="C772" s="10">
+        <v>0</v>
+      </c>
+      <c r="D772" s="10">
+        <v>0</v>
+      </c>
+      <c r="E772" s="10">
+        <v>0</v>
+      </c>
+      <c r="F772" s="10">
+        <v>0</v>
+      </c>
+      <c r="G772" s="10">
+        <v>301</v>
+      </c>
+      <c r="H772" s="10">
+        <v>7</v>
+      </c>
+      <c r="I772" s="10">
+        <v>5</v>
+      </c>
+      <c r="J772" s="10">
+        <v>0</v>
+      </c>
+      <c r="K772" s="10">
+        <v>57</v>
+      </c>
+      <c r="L772" s="10">
+        <v>0</v>
+      </c>
+      <c r="M772" s="10">
+        <v>0</v>
+      </c>
+      <c r="N772" s="10">
+        <v>4</v>
+      </c>
+      <c r="O772" s="10">
+        <v>315</v>
+      </c>
+      <c r="P772" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="773" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A773" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="B773" s="10">
+        <v>305</v>
+      </c>
+      <c r="C773" s="10">
+        <v>0</v>
+      </c>
+      <c r="D773" s="10">
+        <v>0</v>
+      </c>
+      <c r="E773" s="10">
+        <v>0</v>
+      </c>
+      <c r="F773" s="10">
+        <v>0</v>
+      </c>
+      <c r="G773" s="10">
+        <v>305</v>
+      </c>
+      <c r="H773" s="10">
+        <v>7</v>
+      </c>
+      <c r="I773" s="10">
+        <v>3</v>
+      </c>
+      <c r="J773" s="10">
+        <v>0</v>
+      </c>
+      <c r="K773" s="10">
+        <v>53</v>
+      </c>
+      <c r="L773" s="10">
+        <v>0</v>
+      </c>
+      <c r="M773" s="10">
+        <v>0</v>
+      </c>
+      <c r="N773" s="10">
+        <v>13</v>
+      </c>
+      <c r="O773" s="10">
+        <v>305</v>
+      </c>
+      <c r="P773" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="774" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A774" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="B774" s="10"/>
+      <c r="C774" s="10"/>
+      <c r="D774" s="10"/>
+      <c r="E774" s="10"/>
+      <c r="F774" s="10"/>
+      <c r="G774" s="10"/>
+      <c r="H774" s="10"/>
+      <c r="I774" s="10"/>
+      <c r="J774" s="10"/>
+      <c r="K774" s="10"/>
+      <c r="L774" s="10"/>
+      <c r="M774" s="10"/>
+      <c r="N774" s="10"/>
+      <c r="O774" s="10"/>
+      <c r="P774" s="11"/>
+    </row>
+    <row r="775" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A775" s="12" t="s">
+        <v>788</v>
+      </c>
+      <c r="B775" s="13"/>
+      <c r="C775" s="13"/>
+      <c r="D775" s="13"/>
+      <c r="E775" s="13"/>
+      <c r="F775" s="13"/>
+      <c r="G775" s="13"/>
+      <c r="H775" s="13"/>
+      <c r="I775" s="13"/>
+      <c r="J775" s="13"/>
+      <c r="K775" s="13"/>
+      <c r="L775" s="13"/>
+      <c r="M775" s="13"/>
+      <c r="N775" s="13"/>
+      <c r="O775" s="13"/>
+      <c r="P775" s="14"/>
+    </row>
+    <row r="776" spans="1:16" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>